<commit_message>
Finish Usage on DWH
</commit_message>
<xml_diff>
--- a/Pipelines.xlsx
+++ b/Pipelines.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25831"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25928"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\asus\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\TC Data\spvb-spp\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5309887-0F15-498E-8DE5-CF5B1C859370}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8F7217F-91F7-4BA6-9F00-9E0A1A5B80D6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="690" yWindow="-120" windowWidth="28230" windowHeight="16440" xr2:uid="{88225B27-141A-434B-A386-CDC74F3A8DCF}"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="46272" windowHeight="25392" xr2:uid="{88225B27-141A-434B-A386-CDC74F3A8DCF}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="11">
   <si>
     <t>SAP</t>
   </si>
@@ -415,7 +415,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme 2013 - 2022" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -426,7 +426,7 @@
   <dimension ref="D3:H6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I15" sqref="I15"/>
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -467,14 +467,16 @@
       </c>
       <c r="H4" s="1"/>
     </row>
-    <row r="5" spans="4:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="5" spans="4:8" ht="45" x14ac:dyDescent="0.25">
       <c r="D5" s="1" t="s">
         <v>1</v>
       </c>
       <c r="F5" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="G5" s="1"/>
+      <c r="G5" s="1" t="s">
+        <v>7</v>
+      </c>
       <c r="H5" s="1"/>
     </row>
     <row r="6" spans="4:8" x14ac:dyDescent="0.25">

</xml_diff>